<commit_message>
V1.00 As built by PCBway, Aug 7, 2024
</commit_message>
<xml_diff>
--- a/PocketFT8XcvrHW/PTHComponents.xlsx
+++ b/PocketFT8XcvrHW/PTHComponents.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jconrad/GitHub/PocketFT8Xcvr/hw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jconrad/GitHub/PocketFT8Xcvr/PocketFT8XcvrHW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676CAD20-2EB0-E54D-85C7-9CCCB94412DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CF7AC9-9F44-4445-8F47-175546CB6433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="3560" windowWidth="16320" windowHeight="17740" xr2:uid="{75A7EE58-9EAC-8E47-8DE8-A7442901E7FD}"/>
+    <workbookView xWindow="1420" yWindow="780" windowWidth="20460" windowHeight="17740" xr2:uid="{75A7EE58-9EAC-8E47-8DE8-A7442901E7FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
   <si>
     <t>Item</t>
   </si>
@@ -151,12 +151,6 @@
     <t>2.54 mm</t>
   </si>
   <si>
-    <t>RG174</t>
-  </si>
-  <si>
-    <t>Antenna cable assembly</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -203,6 +197,24 @@
   </si>
   <si>
     <t>44PF</t>
+  </si>
+  <si>
+    <t>20-pin 2.54mm pitch tall female header</t>
+  </si>
+  <si>
+    <t>RG316</t>
+  </si>
+  <si>
+    <t>Antenna pigtail</t>
+  </si>
+  <si>
+    <t>amazon</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>dk</t>
   </si>
 </sst>
 </file>
@@ -604,13 +616,13 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="9.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="43.5" customWidth="1"/>
@@ -630,7 +642,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
@@ -643,8 +655,11 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>8</v>
@@ -658,11 +673,14 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -691,6 +709,9 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
@@ -706,6 +727,9 @@
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
@@ -740,7 +764,7 @@
         <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>26</v>
@@ -758,7 +782,7 @@
         <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>26</v>
@@ -787,11 +811,14 @@
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D11" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>31</v>
@@ -805,11 +832,14 @@
       <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D12" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>31</v>
@@ -823,11 +853,14 @@
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D13" t="s">
         <v>32</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>31</v>
@@ -841,11 +874,14 @@
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D14" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>31</v>
@@ -872,13 +908,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -887,13 +923,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -902,13 +938,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -917,13 +956,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -938,10 +980,10 @@
         <v>25</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -956,10 +998,10 @@
         <v>25</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -970,11 +1012,14 @@
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>31</v>
@@ -988,11 +1033,14 @@
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>31</v>
@@ -1006,11 +1054,14 @@
       <c r="B24" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>31</v>
@@ -1024,11 +1075,14 @@
       <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="C25" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Housecleaning after abandoning the QFN16 SI5351 package
</commit_message>
<xml_diff>
--- a/PocketFT8XcvrHW/PTHComponents.xlsx
+++ b/PocketFT8XcvrHW/PTHComponents.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jconrad/GitHub/PocketFT8Xcvr/PocketFT8XcvrHW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jconrad/GitHub/PocketFT8Xcvr/hw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CF7AC9-9F44-4445-8F47-175546CB6433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676CAD20-2EB0-E54D-85C7-9CCCB94412DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="780" windowWidth="20460" windowHeight="17740" xr2:uid="{75A7EE58-9EAC-8E47-8DE8-A7442901E7FD}"/>
+    <workbookView xWindow="1420" yWindow="3560" windowWidth="16320" windowHeight="17740" xr2:uid="{75A7EE58-9EAC-8E47-8DE8-A7442901E7FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
   <si>
     <t>Item</t>
   </si>
@@ -151,6 +151,12 @@
     <t>2.54 mm</t>
   </si>
   <si>
+    <t>RG174</t>
+  </si>
+  <si>
+    <t>Antenna cable assembly</t>
+  </si>
+  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -197,24 +203,6 @@
   </si>
   <si>
     <t>44PF</t>
-  </si>
-  <si>
-    <t>20-pin 2.54mm pitch tall female header</t>
-  </si>
-  <si>
-    <t>RG316</t>
-  </si>
-  <si>
-    <t>Antenna pigtail</t>
-  </si>
-  <si>
-    <t>amazon</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>dk</t>
   </si>
 </sst>
 </file>
@@ -616,13 +604,13 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="43.5" customWidth="1"/>
@@ -642,7 +630,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
@@ -655,11 +643,8 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>8</v>
@@ -673,14 +658,11 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -709,9 +691,6 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
@@ -727,9 +706,6 @@
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
@@ -764,7 +740,7 @@
         <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>26</v>
@@ -782,7 +758,7 @@
         <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>26</v>
@@ -811,14 +787,11 @@
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D11" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>31</v>
@@ -832,14 +805,11 @@
       <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D12" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>31</v>
@@ -853,14 +823,11 @@
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D13" t="s">
         <v>32</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>31</v>
@@ -874,14 +841,11 @@
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D14" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>31</v>
@@ -908,13 +872,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -923,13 +887,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -938,16 +902,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -956,16 +917,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -980,10 +938,10 @@
         <v>25</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -998,10 +956,10 @@
         <v>25</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1012,14 +970,11 @@
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>31</v>
@@ -1033,14 +988,11 @@
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>31</v>
@@ -1054,14 +1006,11 @@
       <c r="B24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>31</v>
@@ -1075,14 +1024,11 @@
       <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>31</v>

</xml_diff>